<commit_message>
added snapshot test und fixed others
</commit_message>
<xml_diff>
--- a/unittests/test-edi-energy-mirror-repo/edi_energy_de/FV2310/expected-output/2024-03-30_change_histories.xlsx
+++ b/unittests/test-edi-energy-mirror-repo/edi_energy_de/FV2310/expected-output/2024-03-30_change_histories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>Änd-ID</t>
   </si>
@@ -65,6 +65,9 @@
     <t>10000</t>
   </si>
   <si>
+    <t>25216</t>
+  </si>
+  <si>
     <t>23936</t>
   </si>
   <si>
@@ -72,6 +75,9 @@
   </si>
   <si>
     <t>23938</t>
+  </si>
+  <si>
+    <t>Gesamtes Dokument</t>
   </si>
   <si>
     <t>Kapitel 4.1 Anwendungsfälle ORDERS (Übersicht 1), Prüfidentifikator 17202, 17203, DTM+203 Ausführungsdatum</t>
@@ -85,6 +91,9 @@
   <si>
     <t xml:space="preserve">Version: 2.2b
 </t>
+  </si>
+  <si>
+    <t>Fünfstelliger Segmentzähler nicht vorhanden</t>
   </si>
   <si>
     <t>Muss [33] ∨ [34]
@@ -97,6 +106,9 @@
 </t>
   </si>
   <si>
+    <t>Fünfstelliger Segmentzähler vorhanden</t>
+  </si>
+  <si>
     <t>Muss [33] ⊻ [34]
 Bedingung: 
 [33] Wenn IMD+Z01 vorhanden
@@ -106,10 +118,16 @@
     <t>Version AHB aktualisiert. Zusätzlich wurden Schreibfehler, Layout, Struktur etc. geändert, die keinen Einfluss auf die inhaltliche Aussage haben.</t>
   </si>
   <si>
+    <t>Anpassung an das Layout der Konsultationsergebnisse vom 19. Juni 2024</t>
+  </si>
+  <si>
     <t>Nutzung des korrekten Operators zwischen den Voraussetzungen.</t>
   </si>
   <si>
     <t>Genehmigt</t>
+  </si>
+  <si>
+    <t>Anpassung (26.07.2024)</t>
   </si>
   <si>
     <t xml:space="preserve">	24589</t>
@@ -636,7 +654,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -677,16 +695,16 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -697,19 +715,19 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -720,19 +738,19 @@
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -743,19 +761,42 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -803,22 +844,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -826,22 +867,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -849,22 +890,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: parsing of segment ids (#406)
* new filter in edifact structure cell

* add segment_id parsing

* add segment_id where it belongs

* fixed / added tests

* added snapshot test und fixed others

* fixed tests

* fixed snapshot test

* fix minor issue

* update snapshot

* updated snapshot final

* updated gitignore

* snapshot final 2

---------

Co-authored-by: kevin <68426071+hf-krechan@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/unittests/test-edi-energy-mirror-repo/edi_energy_de/FV2310/expected-output/2024-03-30_change_histories.xlsx
+++ b/unittests/test-edi-energy-mirror-repo/edi_energy_de/FV2310/expected-output/2024-03-30_change_histories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>Änd-ID</t>
   </si>
@@ -65,6 +65,9 @@
     <t>10000</t>
   </si>
   <si>
+    <t>25216</t>
+  </si>
+  <si>
     <t>23936</t>
   </si>
   <si>
@@ -72,6 +75,9 @@
   </si>
   <si>
     <t>23938</t>
+  </si>
+  <si>
+    <t>Gesamtes Dokument</t>
   </si>
   <si>
     <t>Kapitel 4.1 Anwendungsfälle ORDERS (Übersicht 1), Prüfidentifikator 17202, 17203, DTM+203 Ausführungsdatum</t>
@@ -85,6 +91,9 @@
   <si>
     <t xml:space="preserve">Version: 2.2b
 </t>
+  </si>
+  <si>
+    <t>Fünfstelliger Segmentzähler nicht vorhanden</t>
   </si>
   <si>
     <t>Muss [33] ∨ [34]
@@ -97,6 +106,9 @@
 </t>
   </si>
   <si>
+    <t>Fünfstelliger Segmentzähler vorhanden</t>
+  </si>
+  <si>
     <t>Muss [33] ⊻ [34]
 Bedingung: 
 [33] Wenn IMD+Z01 vorhanden
@@ -106,10 +118,16 @@
     <t>Version AHB aktualisiert. Zusätzlich wurden Schreibfehler, Layout, Struktur etc. geändert, die keinen Einfluss auf die inhaltliche Aussage haben.</t>
   </si>
   <si>
+    <t>Anpassung an das Layout der Konsultationsergebnisse vom 19. Juni 2024</t>
+  </si>
+  <si>
     <t>Nutzung des korrekten Operators zwischen den Voraussetzungen.</t>
   </si>
   <si>
     <t>Genehmigt</t>
+  </si>
+  <si>
+    <t>Anpassung (26.07.2024)</t>
   </si>
   <si>
     <t xml:space="preserve">	24589</t>
@@ -636,7 +654,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -677,16 +695,16 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -697,19 +715,19 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -720,19 +738,19 @@
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -743,19 +761,42 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -803,22 +844,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -826,22 +867,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -849,22 +890,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update expected xlsx for change history
</commit_message>
<xml_diff>
--- a/unittests/test-edi-energy-mirror-repo/edi_energy_de/FV2310/expected-output/2024-03-30_change_histories.xlsx
+++ b/unittests/test-edi-energy-mirror-repo/edi_energy_de/FV2310/expected-output/2024-03-30_change_histories.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="COMDISAHB" sheetId="1" r:id="rId1"/>
-    <sheet name="ORDERSORDRSPAHBMaBiS" sheetId="2" r:id="rId2"/>
-    <sheet name="PARTINAHB" sheetId="3" r:id="rId3"/>
+    <sheet name="AHB_COMDIS_1.0d" sheetId="1" r:id="rId1"/>
+    <sheet name="AHB_ORDRSP_2.2c" sheetId="2" r:id="rId2"/>
+    <sheet name="AHB_PARTIN_1.0c" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>